<commit_message>
update BrandstofTypeRepo: voegToe, Update, Bestaat
VoegBranstoftypeToe returned nu het gemaakte BrandstofType
</commit_message>
<xml_diff>
--- a/Documentatie/Logboeken/TaakVerdeling.xlsx
+++ b/Documentatie/Logboeken/TaakVerdeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project Fleet\Documentatie\Logboeken\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC530CB3-CC7E-4872-9A7F-82BBA0330705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE039FC-DB10-48B6-8214-0236021EC07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B4D898-FE95-45D7-8787-EBF54F774182}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
   <si>
     <t>Uitvoerder</t>
   </si>
@@ -471,46 +471,46 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -859,7 +859,7 @@
   <dimension ref="B3:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B16" zoomScale="92" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,19 +877,19 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="50" t="s">
+      <c r="L3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="50"/>
+      <c r="M3" s="40"/>
     </row>
     <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E4" s="3" t="s">
@@ -915,16 +915,16 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="43" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="42">
         <v>44476</v>
       </c>
       <c r="I5" s="15" t="s">
@@ -938,12 +938,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="44"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="45"/>
       <c r="G6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="52"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="15" t="s">
         <v>11</v>
       </c>
@@ -955,14 +955,14 @@
       </c>
     </row>
     <row r="7" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="44"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="32" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="52"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="15" t="s">
         <v>11</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="G8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="52"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="15" t="s">
         <v>11</v>
       </c>
@@ -1004,7 +1004,7 @@
       <c r="G9" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="52"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="15" t="s">
         <v>22</v>
       </c>
@@ -1012,16 +1012,16 @@
       <c r="M9" s="19"/>
     </row>
     <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="46" t="s">
         <v>31</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="49">
         <v>44483</v>
       </c>
       <c r="I10" s="17" t="s">
@@ -1031,12 +1031,12 @@
       <c r="M10" s="19"/>
     </row>
     <row r="11" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="53"/>
-      <c r="F11" s="49"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="47"/>
       <c r="G11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="47"/>
+      <c r="H11" s="50"/>
       <c r="I11" s="20" t="s">
         <v>11</v>
       </c>
@@ -1044,12 +1044,12 @@
       <c r="M11" s="19"/>
     </row>
     <row r="12" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="41"/>
-      <c r="F12" s="43"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="48"/>
       <c r="G12" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="47"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="20" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="G13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="47"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="17" t="s">
         <v>11</v>
       </c>
@@ -1083,7 +1083,7 @@
       <c r="G14" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="47"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="17" t="s">
         <v>11</v>
       </c>
@@ -1091,27 +1091,27 @@
       <c r="M14" s="31"/>
     </row>
     <row r="15" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="46" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="48"/>
+      <c r="H15" s="51"/>
       <c r="I15" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="45"/>
-      <c r="F16" s="43"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="48"/>
       <c r="G16" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="46">
+      <c r="H16" s="49">
         <v>44490</v>
       </c>
       <c r="I16" s="13" t="s">
@@ -1119,53 +1119,53 @@
       </c>
     </row>
     <row r="17" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="46" t="s">
         <v>43</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="47"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="45"/>
-      <c r="F18" s="43"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="48"/>
       <c r="G18" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="47"/>
+      <c r="H18" s="50"/>
       <c r="I18" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="46" t="s">
         <v>45</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="47"/>
+      <c r="H19" s="50"/>
       <c r="I19" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="44"/>
-      <c r="F20" s="43"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="48"/>
       <c r="G20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="47"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="23" t="s">
         <v>11</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="G21" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="48"/>
+      <c r="H21" s="51"/>
       <c r="I21" s="23" t="s">
         <v>11</v>
       </c>
@@ -1190,16 +1190,16 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="46" t="s">
         <v>7</v>
       </c>
       <c r="G22" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="49">
         <v>44497</v>
       </c>
       <c r="I22" s="27" t="s">
@@ -1209,12 +1209,12 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="5:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="41"/>
-      <c r="F23" s="49"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="47"/>
       <c r="G23" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="47"/>
+      <c r="H23" s="50"/>
       <c r="I23" s="27"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1223,11 +1223,11 @@
       <c r="E24" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="49"/>
+      <c r="F24" s="47"/>
       <c r="G24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="47"/>
+      <c r="H24" s="50"/>
       <c r="I24" s="27" t="s">
         <v>11</v>
       </c>
@@ -1238,11 +1238,11 @@
       <c r="E25" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="49"/>
+      <c r="F25" s="47"/>
       <c r="G25" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="H25" s="47"/>
+      <c r="H25" s="50"/>
       <c r="I25" s="27" t="s">
         <v>11</v>
       </c>
@@ -1253,11 +1253,11 @@
       <c r="E26" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="49"/>
+      <c r="F26" s="47"/>
       <c r="G26" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="47"/>
+      <c r="H26" s="50"/>
       <c r="I26" s="27" t="s">
         <v>11</v>
       </c>
@@ -1268,11 +1268,11 @@
       <c r="E27" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="49"/>
+      <c r="F27" s="47"/>
       <c r="G27" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="47"/>
+      <c r="H27" s="50"/>
       <c r="I27" s="29" t="s">
         <v>11</v>
       </c>
@@ -1283,11 +1283,11 @@
       <c r="E28" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="43"/>
+      <c r="F28" s="48"/>
       <c r="G28" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="48"/>
+      <c r="H28" s="51"/>
       <c r="I28" s="29" t="s">
         <v>11</v>
       </c>
@@ -1303,7 +1303,9 @@
         <v>55</v>
       </c>
       <c r="H29" s="39"/>
-      <c r="I29" s="38"/>
+      <c r="I29" s="38" t="s">
+        <v>10</v>
+      </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
@@ -1369,13 +1371,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="H5:H9"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="H10:H15"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="E5:E7"/>
@@ -1387,6 +1382,13 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F22:F28"/>
     <mergeCell ref="H22:H28"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="H5:H9"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="H10:H15"/>
   </mergeCells>
   <conditionalFormatting sqref="I5:I35">
     <cfRule type="expression" dxfId="3" priority="1">

</xml_diff>